<commit_message>
Commit containing updated procedures, surface measuremnts, and reports.
</commit_message>
<xml_diff>
--- a/Fiducial Worksheet Transforms_6.12.17.xlsx
+++ b/Fiducial Worksheet Transforms_6.12.17.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Owner\Documents\MOSES\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Owner\Documents\MOSES\MOSES3_OpticalTesting\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -549,7 +549,7 @@
   <dimension ref="A1:I6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J11" sqref="J11"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -594,7 +594,7 @@
         <v>-0.98</v>
       </c>
       <c r="C2">
-        <v>-2.2599999999999998</v>
+        <v>-2.27</v>
       </c>
       <c r="D2">
         <v>-1.28</v>
@@ -608,7 +608,7 @@
         <v>1.3</v>
       </c>
       <c r="C3">
-        <v>0.31</v>
+        <v>0.28999999999999998</v>
       </c>
       <c r="D3">
         <v>-0.96</v>
@@ -622,7 +622,7 @@
         <v>88.49</v>
       </c>
       <c r="C4">
-        <v>-179.83</v>
+        <v>-179.65</v>
       </c>
       <c r="D4">
         <v>-91.74</v>
@@ -636,7 +636,7 @@
         <v>1.04</v>
       </c>
       <c r="C5">
-        <v>1.01</v>
+        <v>1</v>
       </c>
       <c r="D5">
         <v>0.99</v>

</xml_diff>